<commit_message>
Removed column "ChangeOfTypeScale" from command "Relationships"
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/15_graph_solver_euro_example.xlsx
+++ b/backend_tests/z_input_files/v2/15_graph_solver_euro_example.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="195">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -514,13 +514,7 @@
     <t xml:space="preserve">DestinationInterface</t>
   </si>
   <si>
-    <t xml:space="preserve">RelativeInterfaces</t>
-  </si>
-  <si>
     <t xml:space="preserve">RelationType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChangeOfTypeScale</t>
   </si>
   <si>
     <t xml:space="preserve">Weight</t>
@@ -1008,22 +1002,22 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>135</v>
@@ -1178,19 +1172,19 @@
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,7 +1195,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>42</v>
@@ -1210,10 +1204,10 @@
         <v>42</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,7 +1218,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>42</v>
@@ -1236,7 +1230,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1241,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>42</v>
@@ -1259,7 +1253,7 @@
         <v>39</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,7 +1264,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>42</v>
@@ -1279,10 +1273,10 @@
         <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,7 +1287,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>42</v>
@@ -1302,10 +1296,10 @@
         <v>42</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,7 +1310,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>42</v>
@@ -1328,7 +1322,7 @@
         <v>36</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1339,7 +1333,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>42</v>
@@ -1351,7 +1345,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1362,7 +1356,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>43</v>
@@ -1371,10 +1365,10 @@
         <v>43</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,7 +1379,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>43</v>
@@ -1394,10 +1388,10 @@
         <v>43</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,7 +1402,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>43</v>
@@ -1417,10 +1411,10 @@
         <v>43</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,7 +1425,7 @@
         <v>111</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>43</v>
@@ -1443,7 +1437,7 @@
         <v>111</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,7 +1448,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -1466,7 +1460,7 @@
         <v>34</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,7 +1471,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>43</v>
@@ -1489,7 +1483,7 @@
         <v>35</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,7 +3043,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3285,7 +3279,7 @@
   </sheetPr>
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -6485,7 +6479,7 @@
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6494,15 +6488,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="22.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="17.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="15.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="12" style="4" width="15.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="10" style="4" width="15.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6518,7 +6510,7 @@
       <c r="D1" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="5" t="s">
         <v>161</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -6531,14 +6523,10 @@
         <v>164</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6555,10 +6543,7 @@
         <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6575,10 +6560,7 @@
         <v>75</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6595,10 +6577,7 @@
         <v>80</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6615,10 +6594,7 @@
         <v>78</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6635,10 +6611,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6655,10 +6628,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6675,10 +6645,7 @@
         <v>36</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6695,10 +6662,7 @@
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6715,10 +6679,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6735,16 +6696,12 @@
         <v>39</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>167</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
@@ -6759,8 +6716,8 @@
       <c r="D12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>167</v>
+      <c r="E12" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6776,8 +6733,8 @@
       <c r="D13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>167</v>
+      <c r="E13" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6793,8 +6750,8 @@
       <c r="D14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>167</v>
+      <c r="E14" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6810,8 +6767,8 @@
       <c r="D15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>167</v>
+      <c r="E15" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6827,8 +6784,8 @@
       <c r="D16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>167</v>
+      <c r="E16" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6844,8 +6801,8 @@
       <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>167</v>
+      <c r="E17" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6861,15 +6818,13 @@
       <c r="D18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9" t="s">
-        <v>167</v>
-      </c>
+      <c r="E18" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
@@ -6884,11 +6839,11 @@
       <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>168</v>
+      <c r="E19" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6904,11 +6859,11 @@
       <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="E20" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6924,8 +6879,8 @@
       <c r="D21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>167</v>
+      <c r="E21" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6941,8 +6896,8 @@
       <c r="D22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>167</v>
+      <c r="E22" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6958,10 +6913,10 @@
       <c r="D23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="H23" s="13" t="s">
+      <c r="E23" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6978,10 +6933,10 @@
       <c r="D24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="H24" s="0" t="s">
+      <c r="E24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solver change to handle ScaleChanges and BackInterfaces.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/15_graph_solver_euro_example.xlsx
+++ b/backend_tests/z_input_files/v2/15_graph_solver_euro_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="200">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -687,7 +687,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,8 +696,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFBCE4E5"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEDCC6"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -742,7 +754,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -799,7 +811,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -807,19 +827,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -857,7 +889,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFBCE4E5"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -873,7 +905,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFEDCC6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1026,10 +1058,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1068,10 +1100,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>138</v>
@@ -1083,15 +1115,15 @@
         <v>46</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>138</v>
@@ -1103,24 +1135,24 @@
         <v>46</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>138</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0.3</v>
@@ -1128,10 +1160,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>138</v>
@@ -1143,15 +1175,15 @@
         <v>45</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>138</v>
@@ -1163,48 +1195,51 @@
         <v>45</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>0.6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="n">
-        <v>0.9</v>
+      <c r="C8" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,7 +1247,7 @@
         <v>110</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>179</v>
@@ -1224,10 +1259,10 @@
         <v>45</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,7 +1270,7 @@
         <v>110</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>179</v>
@@ -1247,56 +1282,56 @@
         <v>45</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>182</v>
+        <v>41</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>181</v>
+      <c r="D11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="A12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>184</v>
+      <c r="D12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1304,7 +1339,7 @@
         <v>111</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>179</v>
@@ -1316,10 +1351,10 @@
         <v>45</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,7 +1362,7 @@
         <v>111</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>179</v>
@@ -1339,56 +1374,56 @@
         <v>45</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>187</v>
+        <v>39</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>189</v>
+      <c r="D15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="A16" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>190</v>
+      <c r="D16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,7 +1431,7 @@
         <v>112</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>179</v>
@@ -1408,10 +1443,10 @@
         <v>46</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,7 +1454,7 @@
         <v>112</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>179</v>
@@ -1431,10 +1466,10 @@
         <v>46</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,7 +1477,7 @@
         <v>112</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>179</v>
@@ -1454,10 +1489,10 @@
         <v>46</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>195</v>
+        <v>114</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,7 +1500,7 @@
         <v>112</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>179</v>
@@ -1477,116 +1512,93 @@
         <v>46</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>198</v>
+      <c r="F21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="5" t="n">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="5" t="n">
+      <c r="G24" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1609,7 +1621,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2493,7 +2505,7 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3149,27 +3161,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
         <v>132</v>
       </c>
@@ -3368,6 +3380,39 @@
       </c>
       <c r="I12" s="0" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -3386,10 +3431,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V57"/>
+  <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4079,6 +4126,12 @@
       <c r="G48" s="5" t="s">
         <v>155</v>
       </c>
+      <c r="L48" s="5" t="n">
+        <v>407740.95</v>
+      </c>
+      <c r="S48" s="5" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="5" t="s">
@@ -4179,6 +4232,48 @@
         <v>119</v>
       </c>
       <c r="G57" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14" t="s">
         <v>154</v>
       </c>
     </row>
@@ -5581,10 +5676,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ43"/>
+  <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5685,7 +5780,7 @@
       <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>158</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -5708,7 +5803,7 @@
       <c r="B3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>159</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -5768,13 +5863,16 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>154</v>
       </c>
       <c r="L6" s="0" t="n">
@@ -5787,44 +5885,46 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="L7" s="15" t="n">
-        <v>4.7689</v>
-      </c>
-      <c r="R7" s="15" t="s">
+    <row r="7" customFormat="false" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.423619</v>
+      </c>
+      <c r="R7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="15" t="s">
+      <c r="S7" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="AMJ7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>158</v>
+      <c r="C8" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>121</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>0.423619</v>
-      </c>
-      <c r="R8" s="17" t="s">
+        <v>0.198178</v>
+      </c>
+      <c r="R8" s="18" t="s">
         <v>46</v>
       </c>
       <c r="S8" s="0" t="s">
@@ -5833,21 +5933,18 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>121</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>0.198178</v>
-      </c>
-      <c r="R9" s="17" t="s">
+        <v>0.7</v>
+      </c>
+      <c r="R9" s="18" t="s">
         <v>46</v>
       </c>
       <c r="S9" s="0" t="s">
@@ -5856,7 +5953,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>121</v>
@@ -5865,9 +5962,9 @@
         <v>154</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="R10" s="17" t="s">
+        <v>201.02</v>
+      </c>
+      <c r="R10" s="18" t="s">
         <v>46</v>
       </c>
       <c r="S10" s="0" t="s">
@@ -5875,81 +5972,87 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="B11" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20" t="s">
         <v>154</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>201.02</v>
-      </c>
-      <c r="R11" s="17" t="s">
+        <v>1245.42</v>
+      </c>
+      <c r="R11" s="18" t="s">
         <v>46</v>
       </c>
       <c r="S11" s="0" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="5" t="s">
+    <row r="12" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>1245.42</v>
+      <c r="G12" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="L12" s="17" t="n">
+        <v>2.690051</v>
       </c>
       <c r="R12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="S12" s="0" t="s">
+      <c r="S12" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="13" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="L13" s="15" t="n">
-        <v>2.690051</v>
-      </c>
-      <c r="R13" s="15" t="s">
+      <c r="AMJ12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>0.483017507961291</v>
+      </c>
+      <c r="R13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="S13" s="15" t="s">
+      <c r="S13" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>158</v>
+      <c r="C14" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>123</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0.483017507961291</v>
+        <v>0.318721995608352</v>
       </c>
       <c r="R14" s="0" t="s">
         <v>46</v>
@@ -5960,19 +6063,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>123</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0.318721995608352</v>
+        <v>0.7</v>
       </c>
       <c r="R15" s="0" t="s">
         <v>46</v>
@@ -5983,7 +6083,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>123</v>
@@ -5992,7 +6092,7 @@
         <v>154</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>0.7</v>
+        <v>139.440647380989</v>
       </c>
       <c r="R16" s="0" t="s">
         <v>46</v>
@@ -6003,7 +6103,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>123</v>
@@ -6012,7 +6112,7 @@
         <v>154</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>139.440647380989</v>
+        <v>2886.98274968357</v>
       </c>
       <c r="R17" s="0" t="s">
         <v>46</v>
@@ -6021,62 +6121,65 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="5" t="s">
+    <row r="18" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <v>2886.98274968357</v>
-      </c>
-      <c r="R18" s="0" t="s">
+      <c r="G18" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="L18" s="17" t="n">
+        <v>4.94047619047619</v>
+      </c>
+      <c r="R18" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="S18" s="0" t="s">
+      <c r="S18" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="19" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="L19" s="15" t="n">
-        <v>4.94047619047619</v>
-      </c>
-      <c r="R19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="S19" s="15" t="s">
+      <c r="AMJ18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>158</v>
+      <c r="C20" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>125</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>31.1</v>
+        <v>21.2</v>
       </c>
       <c r="R20" s="0" t="s">
         <v>45</v>
@@ -6087,19 +6190,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>125</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>21.2</v>
+        <v>0.7</v>
       </c>
       <c r="R21" s="0" t="s">
         <v>45</v>
@@ -6110,7 +6210,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>125</v>
@@ -6119,7 +6219,7 @@
         <v>154</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>0.7</v>
+        <v>143.0069</v>
       </c>
       <c r="R22" s="0" t="s">
         <v>45</v>
@@ -6130,7 +6230,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>125</v>
@@ -6139,7 +6239,7 @@
         <v>154</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>143.0069</v>
+        <v>562</v>
       </c>
       <c r="R23" s="0" t="s">
         <v>45</v>
@@ -6148,62 +6248,65 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="5" t="s">
+    <row r="24" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="L24" s="0" t="n">
-        <v>562</v>
-      </c>
-      <c r="R24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="S24" s="0" t="s">
+      <c r="G24" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="L24" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="S24" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="25" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="L25" s="15" t="n">
-        <v>15</v>
-      </c>
-      <c r="R25" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="S25" s="15" t="s">
+      <c r="AMJ24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>11.000603</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="S25" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>158</v>
+      <c r="C26" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>11.000603</v>
+        <v>1.1</v>
       </c>
       <c r="R26" s="0" t="s">
         <v>45</v>
@@ -6214,19 +6317,16 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>1.1</v>
+        <v>0.7</v>
       </c>
       <c r="R27" s="0" t="s">
         <v>45</v>
@@ -6237,7 +6337,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>127</v>
@@ -6246,7 +6346,7 @@
         <v>154</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>0.7</v>
+        <v>218.0069</v>
       </c>
       <c r="R28" s="0" t="s">
         <v>45</v>
@@ -6257,7 +6357,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>127</v>
@@ -6266,7 +6366,7 @@
         <v>154</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>218.0069</v>
+        <v>5054</v>
       </c>
       <c r="R29" s="0" t="s">
         <v>45</v>
@@ -6275,62 +6375,65 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="5" t="s">
+    <row r="30" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="G30" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="L30" s="0" t="n">
-        <v>5054</v>
-      </c>
-      <c r="R30" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="S30" s="0" t="s">
+      <c r="G30" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="L30" s="17" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="R30" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="S30" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="31" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="L31" s="15" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="R31" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="S31" s="15" t="s">
+      <c r="AMJ30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>4.388</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="S31" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>158</v>
+      <c r="C32" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>129</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>4.388</v>
+        <v>4.34</v>
       </c>
       <c r="R32" s="0" t="s">
         <v>45</v>
@@ -6341,19 +6444,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>129</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>4.34</v>
+        <v>0.7</v>
       </c>
       <c r="R33" s="0" t="s">
         <v>45</v>
@@ -6364,7 +6464,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>129</v>
@@ -6373,7 +6473,7 @@
         <v>154</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>0.7</v>
+        <v>421.0069</v>
       </c>
       <c r="R34" s="0" t="s">
         <v>45</v>
@@ -6384,7 +6484,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>129</v>
@@ -6393,7 +6493,7 @@
         <v>154</v>
       </c>
       <c r="L35" s="0" t="n">
-        <v>421.0069</v>
+        <v>14662</v>
       </c>
       <c r="R35" s="0" t="s">
         <v>45</v>
@@ -6402,62 +6502,65 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="5" t="s">
+    <row r="36" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G36" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="L36" s="0" t="n">
-        <v>14662</v>
-      </c>
-      <c r="R36" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="S36" s="0" t="s">
+      <c r="G36" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="L36" s="17" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="R36" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="S36" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="37" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="L37" s="15" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="R37" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="S37" s="15" t="s">
+      <c r="AMJ36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>8.69</v>
+      </c>
+      <c r="R37" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="S37" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="14" t="s">
-        <v>158</v>
+      <c r="C38" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>131</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L38" s="0" t="n">
-        <v>8.69</v>
+        <v>2.79</v>
       </c>
       <c r="R38" s="0" t="s">
         <v>45</v>
@@ -6468,19 +6571,16 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>131</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L39" s="0" t="n">
-        <v>2.79</v>
+        <v>0.7</v>
       </c>
       <c r="R39" s="0" t="s">
         <v>45</v>
@@ -6491,7 +6591,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>131</v>
@@ -6500,7 +6600,7 @@
         <v>154</v>
       </c>
       <c r="L40" s="0" t="n">
-        <v>0.7</v>
+        <v>407.0069</v>
       </c>
       <c r="R40" s="0" t="s">
         <v>45</v>
@@ -6511,7 +6611,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>131</v>
@@ -6520,7 +6620,7 @@
         <v>154</v>
       </c>
       <c r="L41" s="0" t="n">
-        <v>407.0069</v>
+        <v>14562</v>
       </c>
       <c r="R41" s="0" t="s">
         <v>45</v>
@@ -6531,7 +6631,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>131</v>
@@ -6540,32 +6640,12 @@
         <v>154</v>
       </c>
       <c r="L42" s="0" t="n">
-        <v>14562</v>
+        <v>3.26</v>
       </c>
       <c r="R42" s="0" t="s">
         <v>45</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="L43" s="0" t="n">
-        <v>3.26</v>
-      </c>
-      <c r="R43" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="S43" s="0" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6585,10 +6665,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ25"/>
+  <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6620,7 +6700,7 @@
       <c r="D1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="22" t="s">
         <v>164</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -6651,7 +6731,7 @@
       <c r="C2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="23" t="s">
         <v>76</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -6671,7 +6751,7 @@
       <c r="C3" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="23" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -6688,7 +6768,7 @@
       <c r="C4" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="23" t="s">
         <v>81</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -6705,7 +6785,7 @@
       <c r="C5" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="23" t="s">
         <v>78</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -6722,7 +6802,7 @@
       <c r="C6" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="23" t="s">
         <v>83</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -6739,7 +6819,7 @@
       <c r="C7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="24" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -6748,16 +6828,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>38</v>
+        <v>121</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>169</v>
@@ -6765,16 +6848,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>123</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>169</v>
@@ -6782,16 +6865,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>40</v>
+        <v>123</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>169</v>
@@ -6799,55 +6882,50 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>41</v>
+        <v>123</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
+      <c r="A12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>169</v>
@@ -6855,50 +6933,55 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="A15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
         <v>169</v>
       </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>169</v>
@@ -6906,16 +6989,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>169</v>
@@ -6923,52 +7006,47 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10" t="s">
+      <c r="A19" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>45</v>
@@ -6976,101 +7054,157 @@
       <c r="F20" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="A22" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10" t="s">
         <v>169</v>
       </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>169</v>
       </c>
+      <c r="G23" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>13</v>
+      <c r="G24" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G25" s="0" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>